<commit_message>
update data loader, add cac 40 data and final results momentum
</commit_message>
<xml_diff>
--- a/results/PureFactorPortfolio_StrategMomentum_2013-01-31_2018-01-31.xlsx
+++ b/results/PureFactorPortfolio_StrategMomentum_2013-01-31_2018-01-31.xlsx
@@ -55,76 +55,76 @@
     <t>Frais de transaction</t>
   </si>
   <si>
-    <t>3.07%</t>
-  </si>
-  <si>
-    <t>0.61%</t>
-  </si>
-  <si>
-    <t>3.29%</t>
-  </si>
-  <si>
-    <t>0.18</t>
-  </si>
-  <si>
-    <t>0.27</t>
-  </si>
-  <si>
-    <t>-7.75%</t>
-  </si>
-  <si>
-    <t>-0.34%</t>
-  </si>
-  <si>
-    <t>-0.47%</t>
+    <t>10.30%</t>
+  </si>
+  <si>
+    <t>1.99%</t>
+  </si>
+  <si>
+    <t>3.54%</t>
+  </si>
+  <si>
+    <t>0.56</t>
+  </si>
+  <si>
+    <t>0.80</t>
+  </si>
+  <si>
+    <t>-8.15%</t>
+  </si>
+  <si>
+    <t>-0.37%</t>
+  </si>
+  <si>
+    <t>-0.51%</t>
   </si>
   <si>
     <t>0.00%</t>
   </si>
   <si>
-    <t>8.77%</t>
-  </si>
-  <si>
-    <t>1.70%</t>
-  </si>
-  <si>
-    <t>3.11%</t>
-  </si>
-  <si>
-    <t>0.55</t>
-  </si>
-  <si>
-    <t>0.81</t>
-  </si>
-  <si>
-    <t>-4.09%</t>
-  </si>
-  <si>
-    <t>-0.32%</t>
-  </si>
-  <si>
-    <t>-0.43%</t>
-  </si>
-  <si>
-    <t>17.42%</t>
-  </si>
-  <si>
-    <t>3.28%</t>
-  </si>
-  <si>
-    <t>3.18%</t>
-  </si>
-  <si>
-    <t>1.03</t>
-  </si>
-  <si>
-    <t>1.51</t>
-  </si>
-  <si>
-    <t>-5.71%</t>
-  </si>
-  <si>
-    <t>-0.45%</t>
+    <t>16.34%</t>
+  </si>
+  <si>
+    <t>3.09%</t>
+  </si>
+  <si>
+    <t>3.62%</t>
+  </si>
+  <si>
+    <t>0.85</t>
+  </si>
+  <si>
+    <t>1.24</t>
+  </si>
+  <si>
+    <t>-5.73%</t>
+  </si>
+  <si>
+    <t>-0.39%</t>
+  </si>
+  <si>
+    <t>24.24%</t>
+  </si>
+  <si>
+    <t>4.46%</t>
+  </si>
+  <si>
+    <t>3.23%</t>
+  </si>
+  <si>
+    <t>1.38</t>
+  </si>
+  <si>
+    <t>2.02</t>
+  </si>
+  <si>
+    <t>-5.20%</t>
+  </si>
+  <si>
+    <t>-0.31%</t>
+  </si>
+  <si>
+    <t>-0.44%</t>
   </si>
 </sst>
 </file>
@@ -516,7 +516,7 @@
         <v>22</v>
       </c>
       <c r="E2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -533,7 +533,7 @@
         <v>23</v>
       </c>
       <c r="E3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -550,7 +550,7 @@
         <v>24</v>
       </c>
       <c r="E4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -567,7 +567,7 @@
         <v>25</v>
       </c>
       <c r="E5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -584,7 +584,7 @@
         <v>26</v>
       </c>
       <c r="E6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -601,7 +601,7 @@
         <v>27</v>
       </c>
       <c r="E7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -618,7 +618,7 @@
         <v>28</v>
       </c>
       <c r="E8" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -632,7 +632,7 @@
         <v>20</v>
       </c>
       <c r="D9" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="E9" t="s">
         <v>36</v>

</xml_diff>